<commit_message>
New data on Sierra-FG
git-svn-id: file://localhost/tmp/svn2git/svn@3106 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/terasort/data/Data_Mapreduce.xlsx
+++ b/papers/terasort/data/Data_Mapreduce.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="440" windowWidth="25600" windowHeight="16060" tabRatio="194" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28920" windowHeight="17560" tabRatio="357"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sierra-FG" sheetId="4" r:id="rId1"/>
+    <sheet name="India-FG" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="old data" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
     <t>Queen Bee</t>
   </si>
@@ -62,27 +63,9 @@
     <t>QB, 64 workers, 10 reduces ,64 mb chunk size ,8 node</t>
   </si>
   <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>time to solution</t>
-  </si>
-  <si>
     <t>QB,8 nodes, 64 workers, 128 MB chunk size, 30 partitions</t>
   </si>
   <si>
-    <t>24.13 minutes</t>
-  </si>
-  <si>
-    <t>sierra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 workers, 64 mb chunk, </t>
-  </si>
-  <si>
-    <t>35.75 minutes</t>
-  </si>
-  <si>
     <t>Cyder</t>
   </si>
   <si>
@@ -125,27 +108,128 @@
     <t>Reduce Phase</t>
   </si>
   <si>
-    <t>old mr</t>
-  </si>
-  <si>
-    <t>new mr</t>
+    <t>Reduce Phase Time</t>
+  </si>
+  <si>
+    <t>All times in minutes</t>
+  </si>
+  <si>
+    <t>8 workers, 64 mb chunk</t>
+  </si>
+  <si>
+    <t>Input data size in mb</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Time to Start workers</t>
+  </si>
+  <si>
+    <t>Chunk size(MB)</t>
+  </si>
+  <si>
+    <t>Map phase Time</t>
+  </si>
+  <si>
+    <t>Chunk phase Time</t>
+  </si>
+  <si>
+    <t>Number of Reduces</t>
+  </si>
+  <si>
+    <t>Varying Number of Reduces</t>
+  </si>
+  <si>
+    <t>Constant Input Data size(1GB),Number of workers=8</t>
+  </si>
+  <si>
+    <t>Varying chunk size</t>
+  </si>
+  <si>
+    <t>Constant chunk size (64), Input size constant(1GB), Number of workers=8</t>
+  </si>
+  <si>
+    <t>Varying Number of Workers</t>
+  </si>
+  <si>
+    <t>Number of workers</t>
+  </si>
+  <si>
+    <t>India old-MR</t>
+  </si>
+  <si>
+    <t>Time to solution</t>
+  </si>
+  <si>
+    <t>Enhanced MR</t>
+  </si>
+  <si>
+    <t>Input Data size</t>
+  </si>
+  <si>
+    <t>Sierra</t>
+  </si>
+  <si>
+    <t>8 reduces</t>
+  </si>
+  <si>
+    <t>Chunk phase(sec)</t>
+  </si>
+  <si>
+    <t>Time to Start workers(sec)</t>
+  </si>
+  <si>
+    <t>Map phase Time(minutes)</t>
+  </si>
+  <si>
+    <t>Reduce Phase Time(minutes)</t>
+  </si>
+  <si>
+    <t>Time to shutdown workers</t>
+  </si>
+  <si>
+    <t>Master  Time to create sesion in advert</t>
+  </si>
+  <si>
+    <t>Number of Chunks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constant chunk size (64), Input size constant(1GB), </t>
+  </si>
+  <si>
+    <t>Varying input Datasize</t>
+  </si>
+  <si>
+    <t>Workload Per Worker in Map Pahse (MB)</t>
+  </si>
+  <si>
+    <t>Workload per worker Reduce Phase(MB) ~</t>
+  </si>
+  <si>
+    <t>64*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constant chunk size(64mb Input size constant(2GB), </t>
+  </si>
+  <si>
+    <t>*some workers might not have assigned</t>
+  </si>
+  <si>
+    <t>Constant Input Data size(512),Number of workers=8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
     </font>
     <font>
       <u/>
@@ -163,16 +247,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -180,31 +318,162 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="19"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="19" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="36"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="37" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="37" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="37" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="35" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="35"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="35" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="35" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="34" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="34" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="35" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="35" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="37" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="37" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="68">
+    <cellStyle name="Explanatory Text" xfId="37" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -213,6 +482,32 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Heading 1" xfId="19" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="34" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="35" builtinId="18"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -221,6 +516,30 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -266,7 +585,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>'old data'!$A$5:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -290,7 +609,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$9</c:f>
+              <c:f>'old data'!$B$5:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -322,7 +641,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>'old data'!$A$5:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -346,7 +665,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$9</c:f>
+              <c:f>'old data'!$C$5:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -378,7 +697,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>'old data'!$A$5:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -402,7 +721,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$9</c:f>
+              <c:f>'old data'!$D$5:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -434,11 +753,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="421070712"/>
-        <c:axId val="424724824"/>
+        <c:axId val="122294696"/>
+        <c:axId val="122297688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="421070712"/>
+        <c:axId val="122294696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -448,12 +767,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424724824"/>
+        <c:crossAx val="122297688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="424724824"/>
+        <c:axId val="122297688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -464,7 +783,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421070712"/>
+        <c:crossAx val="122294696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -499,16 +818,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>40640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>81280</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>386080</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>132080</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -852,358 +1171,429 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P43"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:P9"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="10" max="11" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+    <row r="1" spans="1:11" ht="17" thickBot="1">
+      <c r="A1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" ht="16" thickTop="1">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" ht="46" thickBot="1">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>48</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="53" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" thickTop="1">
       <c r="A5">
         <v>128</v>
       </c>
       <c r="B5">
-        <v>26.22</v>
+        <v>13.35</v>
       </c>
       <c r="C5">
-        <v>15.08</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>10.92</v>
-      </c>
-      <c r="J5" s="1" t="s">
+        <v>9.4670000000000005</v>
+      </c>
+      <c r="E5">
+        <v>3.2330000000000001</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>256</v>
       </c>
       <c r="B6">
-        <v>38.18</v>
+        <v>16.7</v>
       </c>
       <c r="C6">
-        <v>16.53</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>21.65</v>
-      </c>
-      <c r="J6" s="1">
-        <v>128</v>
-      </c>
-      <c r="K6" s="1">
-        <v>44.22</v>
-      </c>
-      <c r="L6">
-        <v>33.92</v>
-      </c>
-      <c r="M6">
-        <v>9.9830000000000005</v>
-      </c>
-      <c r="O6">
-        <v>128</v>
-      </c>
-      <c r="P6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>10.88</v>
+      </c>
+      <c r="E6">
+        <v>5.117</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>512</v>
       </c>
       <c r="B7">
-        <v>67</v>
+        <v>28.5</v>
       </c>
       <c r="C7">
-        <v>23.3</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>43.65</v>
-      </c>
-      <c r="J7" s="1">
-        <v>256</v>
-      </c>
-      <c r="K7" s="1">
-        <v>89.83</v>
-      </c>
-      <c r="L7">
-        <v>67.67</v>
-      </c>
-      <c r="M7">
-        <v>21.82</v>
-      </c>
-      <c r="O7">
-        <v>256</v>
-      </c>
-      <c r="P7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>20.22</v>
+      </c>
+      <c r="E7">
+        <v>7.4829999999999997</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>64</v>
+      </c>
+      <c r="K7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>1024</v>
       </c>
       <c r="B8">
-        <v>134.19999999999999</v>
+        <v>52.22</v>
       </c>
       <c r="C8">
-        <v>46.43</v>
+        <v>28</v>
       </c>
       <c r="D8">
-        <v>87.32</v>
-      </c>
-      <c r="J8" s="1">
-        <v>512</v>
-      </c>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:16">
+        <v>37.97</v>
+      </c>
+      <c r="E8">
+        <v>13.22</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>128</v>
+      </c>
+      <c r="K8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>2048</v>
       </c>
       <c r="B9">
-        <v>274.3</v>
+        <v>97.45</v>
       </c>
       <c r="C9">
-        <v>96.6</v>
+        <v>50</v>
       </c>
       <c r="D9">
-        <v>177.7</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1024</v>
-      </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
+        <v>75.23</v>
+      </c>
+      <c r="E9">
+        <v>20.78</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <v>256</v>
+      </c>
+      <c r="K9">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="20" thickBot="1">
+      <c r="A15" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="46" thickTop="1">
+      <c r="A16" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="57" thickBot="1">
+      <c r="A17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>108</v>
-      </c>
-      <c r="C13">
-        <v>25.67</v>
-      </c>
-      <c r="D13">
-        <v>81.72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
+      <c r="B18">
+        <v>97.45</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>75.23</v>
+      </c>
+      <c r="E18">
+        <v>20.78</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23">
-        <v>210.6</v>
-      </c>
-      <c r="C23">
-        <v>44.62</v>
-      </c>
-      <c r="D23">
-        <v>164.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26">
-        <v>178.2</v>
-      </c>
-      <c r="C26">
-        <v>38</v>
-      </c>
-      <c r="D26">
-        <v>139.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>30</v>
+      </c>
+      <c r="J18">
+        <v>256</v>
+      </c>
+      <c r="K18">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="20" thickBot="1">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="46" thickTop="1">
+      <c r="A27" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="57" thickBot="1">
+      <c r="A28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32">
-        <v>4</v>
-      </c>
-      <c r="B32">
-        <v>326.10000000000002</v>
-      </c>
-      <c r="C32">
-        <v>45.5</v>
-      </c>
-      <c r="D32">
-        <v>278.8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37">
-        <v>4</v>
-      </c>
-      <c r="B37">
-        <v>421</v>
-      </c>
-      <c r="C37">
-        <v>92</v>
-      </c>
-      <c r="D37">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="B39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41">
-        <v>32</v>
-      </c>
-      <c r="B41">
-        <v>88.62</v>
-      </c>
-      <c r="C41">
-        <v>18.2</v>
-      </c>
-      <c r="D41">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42">
-        <v>64</v>
-      </c>
-      <c r="B42">
-        <v>47.95</v>
-      </c>
-      <c r="C42">
-        <v>18.350000000000001</v>
-      </c>
-      <c r="D42">
-        <v>42.65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43">
         <v>128</v>
       </c>
-      <c r="B43">
-        <v>51</v>
-      </c>
-      <c r="C43">
-        <v>26.4</v>
-      </c>
-      <c r="D43">
-        <v>25</v>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1213,6 +1603,257 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="46" thickTop="1">
+      <c r="A2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20" thickBot="1">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="34" customHeight="1" thickTop="1">
+      <c r="A12" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" thickBot="1">
+      <c r="A13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="20" thickBot="1">
+      <c r="A23" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="46" thickTop="1">
+      <c r="A24" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" thickBot="1">
+      <c r="A25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="3">
+        <v>128</v>
+      </c>
+      <c r="B35" s="3">
+        <v>44.22</v>
+      </c>
+      <c r="C35" s="3">
+        <v>33.92</v>
+      </c>
+      <c r="D35" s="3">
+        <v>9.9830000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3">
+        <v>256</v>
+      </c>
+      <c r="B36" s="3">
+        <v>89.83</v>
+      </c>
+      <c r="C36" s="3">
+        <v>67.67</v>
+      </c>
+      <c r="D36" s="3">
+        <v>21.82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="3">
+        <v>512</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="3">
+        <v>1024</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C5"/>
   <sheetViews>
@@ -1224,37 +1865,37 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1267,46 +1908,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A2:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1315,66 +1945,253 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1">
+    <row r="5" spans="1:4">
+      <c r="A5">
         <v>128</v>
       </c>
-      <c r="B5" s="1">
-        <v>44.22</v>
+      <c r="B5">
+        <v>26.22</v>
       </c>
       <c r="C5">
-        <v>33.92</v>
+        <v>15.08</v>
       </c>
       <c r="D5">
-        <v>9.9830000000000005</v>
-      </c>
-      <c r="F5">
+        <v>10.92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>256</v>
+      </c>
+      <c r="B6">
+        <v>38.18</v>
+      </c>
+      <c r="C6">
+        <v>16.53</v>
+      </c>
+      <c r="D6">
+        <v>21.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>512</v>
+      </c>
+      <c r="B7">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <v>23.3</v>
+      </c>
+      <c r="D7">
+        <v>43.65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>1024</v>
+      </c>
+      <c r="B8">
+        <v>134.19999999999999</v>
+      </c>
+      <c r="C8">
+        <v>46.43</v>
+      </c>
+      <c r="D8">
+        <v>87.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>2048</v>
+      </c>
+      <c r="B9">
+        <v>274.3</v>
+      </c>
+      <c r="C9">
+        <v>96.6</v>
+      </c>
+      <c r="D9">
+        <v>177.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>108</v>
+      </c>
+      <c r="C13">
+        <v>25.67</v>
+      </c>
+      <c r="D13">
+        <v>81.72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>210.6</v>
+      </c>
+      <c r="C23">
+        <v>44.62</v>
+      </c>
+      <c r="D23">
+        <v>164.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>178.2</v>
+      </c>
+      <c r="C26">
+        <v>38</v>
+      </c>
+      <c r="D26">
+        <v>139.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>326.10000000000002</v>
+      </c>
+      <c r="C32">
+        <v>45.5</v>
+      </c>
+      <c r="D32">
+        <v>278.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>421</v>
+      </c>
+      <c r="C37">
+        <v>92</v>
+      </c>
+      <c r="D37">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>88.62</v>
+      </c>
+      <c r="C41">
+        <v>18.2</v>
+      </c>
+      <c r="D41">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>64</v>
+      </c>
+      <c r="B42">
+        <v>47.95</v>
+      </c>
+      <c r="C42">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="D42">
+        <v>42.65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
         <v>128</v>
       </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5">
-        <v>15.33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1">
-        <v>256</v>
-      </c>
-      <c r="B6" s="1">
-        <v>89.83</v>
-      </c>
-      <c r="C6">
-        <v>67.67</v>
-      </c>
-      <c r="D6">
-        <v>21.82</v>
-      </c>
-      <c r="F6">
-        <v>256</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6">
-        <v>19.22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1">
-        <v>512</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1">
-        <v>1024</v>
-      </c>
-      <c r="B8" s="1"/>
+      <c r="B43">
+        <v>51</v>
+      </c>
+      <c r="C43">
+        <v>26.4</v>
+      </c>
+      <c r="D43">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
some more data on svn
git-svn-id: file://localhost/tmp/svn2git/svn@3108 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/terasort/data/Data_Mapreduce.xlsx
+++ b/papers/terasort/data/Data_Mapreduce.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28920" windowHeight="17560" tabRatio="357"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29220" windowHeight="17560" tabRatio="357"/>
   </bookViews>
   <sheets>
     <sheet name="Sierra-FG" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
   <si>
     <t>Queen Bee</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Master  Time to create sesion in advert</t>
   </si>
   <si>
-    <t>Number of Chunks</t>
-  </si>
-  <si>
     <t xml:space="preserve">Constant chunk size (64), Input size constant(1GB), </t>
   </si>
   <si>
@@ -210,13 +207,16 @@
     <t>64*</t>
   </si>
   <si>
-    <t xml:space="preserve">Constant chunk size(64mb Input size constant(2GB), </t>
-  </si>
-  <si>
     <t>*some workers might not have assigned</t>
   </si>
   <si>
-    <t>Constant Input Data size(512),Number of workers=8</t>
+    <t xml:space="preserve">Constant chunk size(64mb Input size constant(2GB), 8 reduces </t>
+  </si>
+  <si>
+    <t>Constant Input Data size(512),Number of workers=8, Number of Reduces=8</t>
+  </si>
+  <si>
+    <t>Time to shutdown workers(sec)</t>
   </si>
 </sst>
 </file>
@@ -361,7 +361,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="68">
+  <cellStyleXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,6 +400,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -472,7 +478,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="68">
+  <cellStyles count="74">
     <cellStyle name="Explanatory Text" xfId="37" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -505,6 +511,9 @@
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="19" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="34" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="35" builtinId="18"/>
@@ -539,6 +548,9 @@
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1171,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1182,15 +1194,14 @@
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="14.1640625" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" customWidth="1"/>
+    <col min="8" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1">
+    <row r="1" spans="1:10" ht="17" thickBot="1">
       <c r="A1" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>46</v>
@@ -1198,7 +1209,7 @@
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="16" thickTop="1">
+    <row r="2" spans="1:10" ht="16" thickTop="1">
       <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
@@ -1208,15 +1219,15 @@
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
     </row>
-    <row r="3" spans="1:11" ht="46" thickBot="1">
+    <row r="3" spans="1:10" ht="46" thickBot="1">
       <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="53" customHeight="1" thickTop="1" thickBot="1">
+      <c r="H3" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="53" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>47</v>
       </c>
@@ -1233,25 +1244,22 @@
         <v>53</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="16" thickTop="1">
+    </row>
+    <row r="5" spans="1:10" ht="16" thickTop="1">
       <c r="A5">
         <v>128</v>
       </c>
@@ -1268,25 +1276,22 @@
         <v>3.2330000000000001</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>10</v>
       </c>
-      <c r="H5">
-        <v>10</v>
+      <c r="H5" t="s">
+        <v>60</v>
       </c>
       <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="J5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>256</v>
       </c>
@@ -1303,25 +1308,22 @@
         <v>5.117</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>10</v>
       </c>
-      <c r="H6">
-        <v>10</v>
+      <c r="H6" t="s">
+        <v>60</v>
       </c>
       <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="J6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>512</v>
       </c>
@@ -1338,25 +1340,22 @@
         <v>7.4829999999999997</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>10</v>
       </c>
       <c r="H7">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="I7">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="J7">
-        <v>64</v>
-      </c>
-      <c r="K7">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>1024</v>
       </c>
@@ -1373,25 +1372,22 @@
         <v>13.22</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>10</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="I8">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="J8">
-        <v>128</v>
-      </c>
-      <c r="K8">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>2048</v>
       </c>
@@ -1408,40 +1404,37 @@
         <v>20.78</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>10</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>256</v>
       </c>
       <c r="I9">
-        <v>30</v>
+        <v>256</v>
       </c>
       <c r="J9">
-        <v>256</v>
-      </c>
-      <c r="K9">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>4096</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="20" thickBot="1">
+    <row r="15" spans="1:10" ht="20" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="46" thickTop="1">
+    <row r="16" spans="1:10" ht="46" thickTop="1">
       <c r="A16" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="57" thickBot="1">
+    <row r="17" spans="1:10" ht="57" thickBot="1">
       <c r="A17" s="7" t="s">
         <v>43</v>
       </c>
@@ -1458,25 +1451,22 @@
         <v>53</v>
       </c>
       <c r="F17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>8</v>
       </c>
@@ -1493,45 +1483,96 @@
         <v>20.78</v>
       </c>
       <c r="F18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G18">
         <v>10</v>
       </c>
       <c r="H18">
-        <v>10</v>
+        <v>256</v>
       </c>
       <c r="I18">
-        <v>30</v>
+        <v>256</v>
       </c>
       <c r="J18">
-        <v>256</v>
-      </c>
-      <c r="K18">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="B19">
+        <v>68.8</v>
+      </c>
+      <c r="C19">
+        <v>51</v>
+      </c>
+      <c r="D19">
+        <v>46.9</v>
+      </c>
+      <c r="E19">
+        <v>20.12</v>
+      </c>
+      <c r="F19">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>128</v>
+      </c>
+      <c r="I19">
+        <v>256</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="20" thickBot="1">
+      <c r="B20">
+        <v>55.18</v>
+      </c>
+      <c r="C20">
+        <v>56</v>
+      </c>
+      <c r="D20">
+        <v>31.97</v>
+      </c>
+      <c r="E20">
+        <v>22.68</v>
+      </c>
+      <c r="F20">
+        <v>25</v>
+      </c>
+      <c r="G20">
+        <v>63</v>
+      </c>
+      <c r="H20">
+        <v>64</v>
+      </c>
+      <c r="I20">
+        <v>256</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="20" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="46" thickTop="1">
+    <row r="27" spans="1:10" ht="61" thickTop="1">
       <c r="A27" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="57" thickBot="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="57" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>34</v>
       </c>
@@ -1548,40 +1589,118 @@
         <v>53</v>
       </c>
       <c r="F28" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="B29">
+        <v>38.58</v>
+      </c>
+      <c r="C29">
+        <v>55</v>
+      </c>
+      <c r="D29">
+        <v>19.75</v>
+      </c>
+      <c r="E29">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>64</v>
+      </c>
+      <c r="I29">
+        <v>64</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="B30">
+        <v>33.270000000000003</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <v>20.12</v>
+      </c>
+      <c r="E30">
+        <v>12.18</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>64</v>
+      </c>
+      <c r="I30">
+        <v>64</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="B31">
+        <v>28.5</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>20.22</v>
+      </c>
+      <c r="E31">
+        <v>7.4829999999999997</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
+      </c>
+      <c r="G31">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>64</v>
+      </c>
+      <c r="I31">
+        <v>64</v>
+      </c>
+      <c r="J31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>128</v>
       </c>
@@ -1688,7 +1807,7 @@
     </row>
     <row r="12" spans="1:6" ht="34" customHeight="1" thickTop="1">
       <c r="A12" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Data with new SAGA-MR
git-svn-id: file://localhost/tmp/svn2git/svn@3154 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/terasort/data/Data_Mapreduce.xlsx
+++ b/papers/terasort/data/Data_Mapreduce.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="274"/>
+    <workbookView xWindow="9160" yWindow="0" windowWidth="26560" windowHeight="16120" tabRatio="274" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sierra-FG" sheetId="4" r:id="rId1"/>
-    <sheet name="India-FG" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sierra-FG" sheetId="4" r:id="rId2"/>
+    <sheet name="India-FG" sheetId="3" r:id="rId3"/>
     <sheet name="old data" sheetId="1" r:id="rId4"/>
+    <sheet name="Sierra_OLD" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="106">
   <si>
     <t>Queen Bee</t>
   </si>
@@ -244,13 +245,109 @@
   </si>
   <si>
     <t>32 reduces, 26 mappers,8 GB Iinput size</t>
+  </si>
+  <si>
+    <t>2 GB</t>
+  </si>
+  <si>
+    <t>1 node</t>
+  </si>
+  <si>
+    <t>8 workers per node</t>
+  </si>
+  <si>
+    <t>Total Time (minutes)</t>
+  </si>
+  <si>
+    <t>Map phase Time (minutes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constant chunk size(64mb Input size constant(4GB), 8 reduces </t>
+  </si>
+  <si>
+    <t>Master  Time to create sesion in advert(sec)</t>
+  </si>
+  <si>
+    <t>64*(2)</t>
+  </si>
+  <si>
+    <t>64*(4)</t>
+  </si>
+  <si>
+    <t>AVG time for 1 Mapper</t>
+  </si>
+  <si>
+    <t>AVG time per 1 Reducer</t>
+  </si>
+  <si>
+    <t>AVG time for 1 Mapper (min)</t>
+  </si>
+  <si>
+    <t>AVG time per 1 Reducer (min)</t>
+  </si>
+  <si>
+    <t>AVG time for 1 Reducer (min)</t>
+  </si>
+  <si>
+    <t>failing in map phase</t>
+  </si>
+  <si>
+    <t>terasort My version</t>
+  </si>
+  <si>
+    <t>QB</t>
+  </si>
+  <si>
+    <t>Input size in GB</t>
+  </si>
+  <si>
+    <t>32 reduces, 64 workers, 256 MB chunk Size</t>
+  </si>
+  <si>
+    <t>But only 29 workers are started</t>
+  </si>
+  <si>
+    <t>39 chunks</t>
+  </si>
+  <si>
+    <t>109 chunks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109 chunks in </t>
+  </si>
+  <si>
+    <t>Input Size (MB)</t>
+  </si>
+  <si>
+    <t>QB , 8 workers, 8 reduces, 256 MB</t>
+  </si>
+  <si>
+    <t>Total Time(Min)</t>
+  </si>
+  <si>
+    <t>32GB(128Mb)</t>
+  </si>
+  <si>
+    <t>6 min b/w each Reducer</t>
+  </si>
+  <si>
+    <t>Second Attempt</t>
+  </si>
+  <si>
+    <t>in Map Phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India </t>
+  </si>
+  <si>
+    <t>2gb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,6 +410,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -337,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -387,8 +507,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFA7BFDE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF95B3D7"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="80">
+  <cellStyleXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -469,8 +607,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="19"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="19" applyAlignment="1">
@@ -514,8 +686,72 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="37" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="36" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="36" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="36" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="36" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="80">
+  <cellStyles count="114">
     <cellStyle name="Explanatory Text" xfId="37" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -554,6 +790,23 @@
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="19" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="34" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="35" builtinId="18"/>
@@ -594,6 +847,23 @@
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -603,6 +873,199 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.073033013368258"/>
+          <c:y val="0.136134453781513"/>
+          <c:w val="0.890136397757583"/>
+          <c:h val="0.801269988310285"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$16:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$K$16:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.27328125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27765625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3385625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$16:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$L$16:$L$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.8025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="702113560"/>
+        <c:axId val="702110648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="702113560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="702110648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="64.0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="702110648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="702113560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -808,11 +1271,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="504821496"/>
-        <c:axId val="504824488"/>
+        <c:axId val="533839736"/>
+        <c:axId val="533842728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="504821496"/>
+        <c:axId val="533839736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,12 +1285,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="504824488"/>
+        <c:crossAx val="533842728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="504824488"/>
+        <c:axId val="533842728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,7 +1301,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="504821496"/>
+        <c:crossAx val="533839736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -870,6 +1333,41 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1226,687 +1724,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" customWidth="1"/>
-    <col min="8" max="9" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" thickBot="1">
-      <c r="A1" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:12" ht="16" thickTop="1">
-      <c r="A2" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:12" ht="46" thickBot="1">
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="53" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="16" thickTop="1">
-      <c r="A5">
-        <v>128</v>
-      </c>
-      <c r="B5">
-        <v>13.35</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>9.4670000000000005</v>
-      </c>
-      <c r="E5">
-        <v>3.2330000000000001</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5">
-        <v>64</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6">
-        <v>256</v>
-      </c>
-      <c r="B6">
-        <v>16.7</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>10.88</v>
-      </c>
-      <c r="E6">
-        <v>5.117</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6">
-        <v>64</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7">
-        <v>512</v>
-      </c>
-      <c r="B7">
-        <v>28.5</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>20.22</v>
-      </c>
-      <c r="E7">
-        <v>7.4829999999999997</v>
-      </c>
-      <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>64</v>
-      </c>
-      <c r="I7">
-        <v>64</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8">
-        <v>1024</v>
-      </c>
-      <c r="B8">
-        <v>52.22</v>
-      </c>
-      <c r="C8">
-        <v>28</v>
-      </c>
-      <c r="D8">
-        <v>37.97</v>
-      </c>
-      <c r="E8">
-        <v>13.22</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>128</v>
-      </c>
-      <c r="I8">
-        <v>128</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="L8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9">
-        <v>2048</v>
-      </c>
-      <c r="B9">
-        <v>97.45</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="D9">
-        <v>75.23</v>
-      </c>
-      <c r="E9">
-        <v>20.78</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9">
-        <v>10</v>
-      </c>
-      <c r="H9">
-        <v>256</v>
-      </c>
-      <c r="I9">
-        <v>256</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9">
-        <v>64.099999999999994</v>
-      </c>
-      <c r="L9">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="20" thickBot="1">
-      <c r="A15" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="46" thickTop="1">
-      <c r="A16" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="57" thickBot="1">
-      <c r="A17" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
-        <v>8</v>
-      </c>
-      <c r="B18">
-        <v>97.45</v>
-      </c>
-      <c r="C18">
-        <v>50</v>
-      </c>
-      <c r="D18">
-        <v>75.23</v>
-      </c>
-      <c r="E18">
-        <v>20.78</v>
-      </c>
-      <c r="F18">
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <v>10</v>
-      </c>
-      <c r="H18">
-        <v>256</v>
-      </c>
-      <c r="I18">
-        <v>256</v>
-      </c>
-      <c r="J18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="B19">
-        <v>68.8</v>
-      </c>
-      <c r="C19">
-        <v>51</v>
-      </c>
-      <c r="D19">
-        <v>46.9</v>
-      </c>
-      <c r="E19">
-        <v>20.12</v>
-      </c>
-      <c r="F19">
-        <v>13</v>
-      </c>
-      <c r="G19">
-        <v>25</v>
-      </c>
-      <c r="H19">
-        <v>128</v>
-      </c>
-      <c r="I19">
-        <v>256</v>
-      </c>
-      <c r="J19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20">
-        <v>27</v>
-      </c>
-      <c r="B20">
-        <v>55.18</v>
-      </c>
-      <c r="C20">
-        <v>56</v>
-      </c>
-      <c r="D20">
-        <v>31.97</v>
-      </c>
-      <c r="E20">
-        <v>22.68</v>
-      </c>
-      <c r="F20">
-        <v>25</v>
-      </c>
-      <c r="G20">
-        <v>63</v>
-      </c>
-      <c r="H20">
-        <v>64</v>
-      </c>
-      <c r="I20">
-        <v>256</v>
-      </c>
-      <c r="J20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21">
-        <v>24</v>
-      </c>
-      <c r="D21">
-        <v>29.4</v>
-      </c>
-      <c r="E21">
-        <v>32.479999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="E22" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="20" thickBot="1">
-      <c r="A26" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="61" thickTop="1">
-      <c r="A27" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="57" thickBot="1">
-      <c r="A28" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29">
-        <v>16</v>
-      </c>
-      <c r="B29">
-        <v>38.58</v>
-      </c>
-      <c r="C29">
-        <v>55</v>
-      </c>
-      <c r="D29">
-        <v>19.75</v>
-      </c>
-      <c r="E29">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="F29">
-        <v>10</v>
-      </c>
-      <c r="G29">
-        <v>10</v>
-      </c>
-      <c r="H29">
-        <v>64</v>
-      </c>
-      <c r="I29">
-        <v>64</v>
-      </c>
-      <c r="J29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30">
-        <v>32</v>
-      </c>
-      <c r="B30">
-        <v>33.270000000000003</v>
-      </c>
-      <c r="C30">
-        <v>28</v>
-      </c>
-      <c r="D30">
-        <v>20.12</v>
-      </c>
-      <c r="E30">
-        <v>12.18</v>
-      </c>
-      <c r="F30">
-        <v>10</v>
-      </c>
-      <c r="G30">
-        <v>10</v>
-      </c>
-      <c r="H30">
-        <v>64</v>
-      </c>
-      <c r="I30">
-        <v>64</v>
-      </c>
-      <c r="J30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31">
-        <v>64</v>
-      </c>
-      <c r="B31">
-        <v>28.5</v>
-      </c>
-      <c r="C31">
-        <v>12</v>
-      </c>
-      <c r="D31">
-        <v>20.22</v>
-      </c>
-      <c r="E31">
-        <v>7.4829999999999997</v>
-      </c>
-      <c r="F31">
-        <v>10</v>
-      </c>
-      <c r="G31">
-        <v>10</v>
-      </c>
-      <c r="H31">
-        <v>64</v>
-      </c>
-      <c r="I31">
-        <v>64</v>
-      </c>
-      <c r="J31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="61" thickBot="1">
-      <c r="A38" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="16" thickTop="1">
-      <c r="A39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40">
-        <v>35.770000000000003</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41">
-        <v>32.729999999999997</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="C45">
-        <v>62</v>
-      </c>
-      <c r="D45">
-        <v>7.133</v>
-      </c>
-      <c r="E45">
-        <v>12.22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46">
-        <v>97.45</v>
-      </c>
-      <c r="C46">
-        <v>50</v>
-      </c>
-      <c r="D46">
-        <v>75.23</v>
-      </c>
-      <c r="E46">
-        <v>20.78</v>
-      </c>
-      <c r="F46">
-        <v>10</v>
-      </c>
-      <c r="G46">
-        <v>10</v>
-      </c>
-      <c r="H46">
-        <v>256</v>
-      </c>
-      <c r="I46">
-        <v>256</v>
-      </c>
-      <c r="J46">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="30">
-      <c r="A53" s="18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55">
-        <v>233.9</v>
-      </c>
-      <c r="D55">
-        <v>99.37</v>
-      </c>
-      <c r="E55">
-        <v>128.80000000000001</v>
+      <c r="B5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1917,10 +1779,1000 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="33" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="10" width="14.1640625" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="17" thickBot="1">
+      <c r="A1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:12" ht="16" thickTop="1">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" ht="46" thickBot="1">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="53" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16" thickTop="1">
+      <c r="A5">
+        <v>128</v>
+      </c>
+      <c r="B5">
+        <v>9.2170000000000005</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5" s="33">
+        <v>2.133</v>
+      </c>
+      <c r="G5">
+        <v>6.2329999999999997</v>
+      </c>
+      <c r="H5">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <f>F5/2</f>
+        <v>1.0665</v>
+      </c>
+      <c r="L5">
+        <f>G7/8</f>
+        <v>1.4775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>256</v>
+      </c>
+      <c r="B6">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6" s="33">
+        <v>2.2330000000000001</v>
+      </c>
+      <c r="G6">
+        <v>7.05</v>
+      </c>
+      <c r="H6">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6">
+        <v>32</v>
+      </c>
+      <c r="K6">
+        <f>F6/4</f>
+        <v>0.55825000000000002</v>
+      </c>
+      <c r="L6">
+        <f>G6/8</f>
+        <v>0.88124999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>512</v>
+      </c>
+      <c r="B7">
+        <v>16.78</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7" s="33">
+        <v>3.8170000000000002</v>
+      </c>
+      <c r="G7">
+        <v>11.82</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>64</v>
+      </c>
+      <c r="J7">
+        <v>64</v>
+      </c>
+      <c r="K7">
+        <f>F7/8</f>
+        <v>0.47712500000000002</v>
+      </c>
+      <c r="L7">
+        <f>G7/8</f>
+        <v>1.4775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>1024</v>
+      </c>
+      <c r="B8">
+        <v>25.62</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8" s="33">
+        <v>4.9169999999999998</v>
+      </c>
+      <c r="G8">
+        <v>19.27</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>128</v>
+      </c>
+      <c r="J8">
+        <v>128</v>
+      </c>
+      <c r="K8">
+        <f>F8/16</f>
+        <v>0.30731249999999999</v>
+      </c>
+      <c r="L8">
+        <f>G8/8</f>
+        <v>2.4087499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>2048</v>
+      </c>
+      <c r="B9">
+        <v>33.770000000000003</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>95</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9" s="33">
+        <v>9.9329999999999998</v>
+      </c>
+      <c r="G9">
+        <v>21.37</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>256</v>
+      </c>
+      <c r="J9">
+        <v>256</v>
+      </c>
+      <c r="K9">
+        <f>F9/32</f>
+        <v>0.31040624999999999</v>
+      </c>
+      <c r="L9">
+        <f>G9/8</f>
+        <v>2.6712500000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>4096</v>
+      </c>
+      <c r="B10">
+        <v>58</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>175</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10" s="33">
+        <v>17.77</v>
+      </c>
+      <c r="G10">
+        <v>36.5</v>
+      </c>
+      <c r="H10">
+        <v>13</v>
+      </c>
+      <c r="I10">
+        <v>512</v>
+      </c>
+      <c r="J10">
+        <v>512</v>
+      </c>
+      <c r="K10">
+        <f>F10/64</f>
+        <v>0.27765624999999999</v>
+      </c>
+      <c r="L10">
+        <f>G10/8</f>
+        <v>4.5625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="20" thickBot="1">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="61" thickTop="1">
+      <c r="A14" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="57" thickBot="1">
+      <c r="A15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>32</v>
+      </c>
+      <c r="C16" s="38">
+        <v>6</v>
+      </c>
+      <c r="D16" s="38">
+        <v>357</v>
+      </c>
+      <c r="E16" s="38">
+        <v>15</v>
+      </c>
+      <c r="F16" s="39">
+        <v>34.979999999999997</v>
+      </c>
+      <c r="G16" s="38">
+        <v>54.42</v>
+      </c>
+      <c r="H16" s="38">
+        <v>13</v>
+      </c>
+      <c r="I16" s="38">
+        <v>512</v>
+      </c>
+      <c r="J16" s="38">
+        <v>512</v>
+      </c>
+      <c r="K16">
+        <f>F16/128</f>
+        <v>0.27328124999999998</v>
+      </c>
+      <c r="L16">
+        <f>G16/8</f>
+        <v>6.8025000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>64</v>
+      </c>
+      <c r="B17">
+        <v>58</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>175</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="F17" s="33">
+        <v>17.77</v>
+      </c>
+      <c r="G17">
+        <v>36.5</v>
+      </c>
+      <c r="H17">
+        <v>13</v>
+      </c>
+      <c r="I17">
+        <v>512</v>
+      </c>
+      <c r="J17">
+        <v>512</v>
+      </c>
+      <c r="K17">
+        <f>F17/64</f>
+        <v>0.27765624999999999</v>
+      </c>
+      <c r="L17">
+        <f>G17/8</f>
+        <v>4.5625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>128</v>
+      </c>
+      <c r="B18">
+        <v>40.17</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>89</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18" s="33">
+        <v>10.92</v>
+      </c>
+      <c r="G18">
+        <v>27</v>
+      </c>
+      <c r="H18">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <v>512</v>
+      </c>
+      <c r="J18">
+        <v>512</v>
+      </c>
+      <c r="K18">
+        <f>F18/32</f>
+        <v>0.34125</v>
+      </c>
+      <c r="L18">
+        <f>G18/8</f>
+        <v>3.375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>256</v>
+      </c>
+      <c r="B19">
+        <v>31.77</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>46</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19" s="33">
+        <v>5.4169999999999998</v>
+      </c>
+      <c r="G19">
+        <v>24.8</v>
+      </c>
+      <c r="H19">
+        <v>13</v>
+      </c>
+      <c r="I19">
+        <v>512</v>
+      </c>
+      <c r="J19">
+        <v>512</v>
+      </c>
+      <c r="K19">
+        <f>F19/16</f>
+        <v>0.33856249999999999</v>
+      </c>
+      <c r="L19">
+        <f>G19/8</f>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>512</v>
+      </c>
+      <c r="B20">
+        <v>31.7</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+      <c r="F20" s="33">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G20">
+        <v>25.9</v>
+      </c>
+      <c r="H20">
+        <v>13</v>
+      </c>
+      <c r="I20">
+        <v>512</v>
+      </c>
+      <c r="J20">
+        <v>512</v>
+      </c>
+      <c r="K20">
+        <f>F20/16</f>
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="L20">
+        <f>G20/8</f>
+        <v>3.2374999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>1024</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="20" thickBot="1">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="46" thickTop="1">
+      <c r="A23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="57" thickBot="1">
+      <c r="A24" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="K24" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="L24" s="35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>58</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>175</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25" s="33">
+        <v>17.77</v>
+      </c>
+      <c r="G25">
+        <v>36.5</v>
+      </c>
+      <c r="H25">
+        <v>13</v>
+      </c>
+      <c r="I25">
+        <v>512</v>
+      </c>
+      <c r="J25">
+        <v>512</v>
+      </c>
+      <c r="K25">
+        <f>F25/32</f>
+        <v>0.55531249999999999</v>
+      </c>
+      <c r="L25">
+        <f>G25/8</f>
+        <v>4.5625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>64</v>
+      </c>
+      <c r="B28">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>115</v>
+      </c>
+      <c r="F28" s="33">
+        <v>27.38</v>
+      </c>
+      <c r="G28">
+        <v>35.03</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="G29" s="17"/>
+    </row>
+    <row r="34" spans="1:12" ht="61" thickBot="1">
+      <c r="A34" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="I34" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J34" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="K34" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="L34" s="35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="16" thickTop="1">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36">
+        <v>35.770000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37">
+        <v>32.729999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38">
+        <v>58</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>175</v>
+      </c>
+      <c r="E38">
+        <v>15</v>
+      </c>
+      <c r="F38" s="33">
+        <v>17.77</v>
+      </c>
+      <c r="G38">
+        <v>36.5</v>
+      </c>
+      <c r="H38">
+        <v>13</v>
+      </c>
+      <c r="I38">
+        <v>512</v>
+      </c>
+      <c r="J38">
+        <v>512</v>
+      </c>
+      <c r="K38">
+        <f>F38/64</f>
+        <v>0.27765624999999999</v>
+      </c>
+      <c r="L38">
+        <f>G38/8</f>
+        <v>4.5625</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="49" thickBot="1">
+      <c r="A49" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="35"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+    </row>
+    <row r="50" spans="1:18" ht="58" thickTop="1" thickBot="1">
+      <c r="A50" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E50" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F50" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G50" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H50" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="I50" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J50" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="K50" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="L50" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="17" thickTop="1">
+      <c r="A51">
+        <v>8</v>
+      </c>
+      <c r="B51" s="40"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+      <c r="L51" s="35"/>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>312.5</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>90</v>
+      </c>
+      <c r="F52" s="33">
+        <v>238.9</v>
+      </c>
+      <c r="G52">
+        <v>70.069999999999993</v>
+      </c>
+      <c r="O52" t="s">
+        <v>94</v>
+      </c>
+      <c r="P52">
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="A53">
+        <v>32</v>
+      </c>
+      <c r="M53" t="s">
+        <v>103</v>
+      </c>
+      <c r="O53" t="s">
+        <v>96</v>
+      </c>
+      <c r="P53">
+        <v>28.67</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>95</v>
+      </c>
+      <c r="R53">
+        <v>38.08</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="A54" t="s">
+        <v>100</v>
+      </c>
+      <c r="F54" s="33">
+        <v>165.3</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="40" customHeight="1">
+      <c r="A57" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
+      <c r="A58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="A59">
+        <v>512</v>
+      </c>
+      <c r="B59">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2154,61 +3006,6 @@
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C5"/>
-  <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="2" spans="1:3">
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2513,4 +3310,702 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="11.83203125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="3"/>
+    <col min="8" max="9" width="14.1640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16" thickBot="1">
+      <c r="A1" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:12" ht="16" thickTop="1">
+      <c r="A2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:12" ht="46" thickBot="1">
+      <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="53" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16" thickTop="1">
+      <c r="A5" s="3">
+        <v>128</v>
+      </c>
+      <c r="B5" s="3">
+        <v>13.35</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>9.4670000000000005</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3.2330000000000001</v>
+      </c>
+      <c r="F5" s="3">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="3">
+        <v>64</v>
+      </c>
+      <c r="J5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3">
+        <v>256</v>
+      </c>
+      <c r="B6" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10.88</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5.117</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="3">
+        <v>64</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3">
+        <v>512</v>
+      </c>
+      <c r="B7" s="3">
+        <v>28.5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3">
+        <v>20.22</v>
+      </c>
+      <c r="E7" s="3">
+        <v>7.4829999999999997</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3">
+        <v>64</v>
+      </c>
+      <c r="I7" s="3">
+        <v>64</v>
+      </c>
+      <c r="J7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3">
+        <v>1024</v>
+      </c>
+      <c r="B8" s="3">
+        <v>52.22</v>
+      </c>
+      <c r="C8" s="3">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>37.97</v>
+      </c>
+      <c r="E8" s="3">
+        <v>13.22</v>
+      </c>
+      <c r="F8" s="3">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3">
+        <v>128</v>
+      </c>
+      <c r="I8" s="3">
+        <v>128</v>
+      </c>
+      <c r="J8" s="3">
+        <v>5</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3">
+        <v>2048</v>
+      </c>
+      <c r="B9" s="3">
+        <v>97.45</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3">
+        <v>75.23</v>
+      </c>
+      <c r="E9" s="3">
+        <v>20.78</v>
+      </c>
+      <c r="F9" s="3">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3">
+        <v>256</v>
+      </c>
+      <c r="I9" s="3">
+        <v>256</v>
+      </c>
+      <c r="J9" s="3">
+        <v>5</v>
+      </c>
+      <c r="K9" s="3">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="L9" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16" thickBot="1">
+      <c r="A15" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="46" thickTop="1">
+      <c r="A16" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="61" thickBot="1">
+      <c r="A17" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3">
+        <v>97.45</v>
+      </c>
+      <c r="C18" s="3">
+        <v>50</v>
+      </c>
+      <c r="D18" s="3">
+        <v>75.23</v>
+      </c>
+      <c r="E18" s="3">
+        <v>20.78</v>
+      </c>
+      <c r="F18" s="3">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3">
+        <v>10</v>
+      </c>
+      <c r="H18" s="3">
+        <v>256</v>
+      </c>
+      <c r="I18" s="3">
+        <v>256</v>
+      </c>
+      <c r="J18" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3">
+        <v>68.8</v>
+      </c>
+      <c r="C19" s="3">
+        <v>51</v>
+      </c>
+      <c r="D19" s="3">
+        <v>46.9</v>
+      </c>
+      <c r="E19" s="3">
+        <v>20.12</v>
+      </c>
+      <c r="F19" s="3">
+        <v>13</v>
+      </c>
+      <c r="G19" s="3">
+        <v>25</v>
+      </c>
+      <c r="H19" s="3">
+        <v>128</v>
+      </c>
+      <c r="I19" s="3">
+        <v>256</v>
+      </c>
+      <c r="J19" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3">
+        <v>27</v>
+      </c>
+      <c r="B20" s="3">
+        <v>55.18</v>
+      </c>
+      <c r="C20" s="3">
+        <v>56</v>
+      </c>
+      <c r="D20" s="3">
+        <v>31.97</v>
+      </c>
+      <c r="E20" s="3">
+        <v>22.68</v>
+      </c>
+      <c r="F20" s="3">
+        <v>25</v>
+      </c>
+      <c r="G20" s="3">
+        <v>63</v>
+      </c>
+      <c r="H20" s="3">
+        <v>64</v>
+      </c>
+      <c r="I20" s="3">
+        <v>256</v>
+      </c>
+      <c r="J20" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3">
+        <v>29.4</v>
+      </c>
+      <c r="E21" s="3">
+        <v>32.479999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="E22" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="16" thickBot="1">
+      <c r="A26" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="61" thickTop="1">
+      <c r="A27" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="61" thickBot="1">
+      <c r="A28" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3">
+        <v>16</v>
+      </c>
+      <c r="B29" s="3">
+        <v>38.58</v>
+      </c>
+      <c r="C29" s="3">
+        <v>55</v>
+      </c>
+      <c r="D29" s="3">
+        <v>19.75</v>
+      </c>
+      <c r="E29" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="F29" s="3">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3">
+        <v>10</v>
+      </c>
+      <c r="H29" s="3">
+        <v>64</v>
+      </c>
+      <c r="I29" s="3">
+        <v>64</v>
+      </c>
+      <c r="J29" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3">
+        <v>32</v>
+      </c>
+      <c r="B30" s="3">
+        <v>33.270000000000003</v>
+      </c>
+      <c r="C30" s="3">
+        <v>28</v>
+      </c>
+      <c r="D30" s="3">
+        <v>20.12</v>
+      </c>
+      <c r="E30" s="3">
+        <v>12.18</v>
+      </c>
+      <c r="F30" s="3">
+        <v>10</v>
+      </c>
+      <c r="G30" s="3">
+        <v>10</v>
+      </c>
+      <c r="H30" s="3">
+        <v>64</v>
+      </c>
+      <c r="I30" s="3">
+        <v>64</v>
+      </c>
+      <c r="J30" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3">
+        <v>64</v>
+      </c>
+      <c r="B31" s="3">
+        <v>28.5</v>
+      </c>
+      <c r="C31" s="3">
+        <v>12</v>
+      </c>
+      <c r="D31" s="3">
+        <v>20.22</v>
+      </c>
+      <c r="E31" s="3">
+        <v>7.4829999999999997</v>
+      </c>
+      <c r="F31" s="3">
+        <v>10</v>
+      </c>
+      <c r="G31" s="3">
+        <v>10</v>
+      </c>
+      <c r="H31" s="3">
+        <v>64</v>
+      </c>
+      <c r="I31" s="3">
+        <v>64</v>
+      </c>
+      <c r="J31" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="61" thickBot="1">
+      <c r="A38" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I38" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="16" thickTop="1">
+      <c r="A39" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="3">
+        <v>35.770000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="3">
+        <v>32.729999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="3">
+        <v>21</v>
+      </c>
+      <c r="C45" s="3">
+        <v>62</v>
+      </c>
+      <c r="D45" s="3">
+        <v>7.133</v>
+      </c>
+      <c r="E45" s="3">
+        <v>12.22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="3">
+        <v>97.45</v>
+      </c>
+      <c r="C46" s="3">
+        <v>50</v>
+      </c>
+      <c r="D46" s="3">
+        <v>75.23</v>
+      </c>
+      <c r="E46" s="3">
+        <v>20.78</v>
+      </c>
+      <c r="F46" s="3">
+        <v>10</v>
+      </c>
+      <c r="G46" s="3">
+        <v>10</v>
+      </c>
+      <c r="H46" s="3">
+        <v>256</v>
+      </c>
+      <c r="I46" s="3">
+        <v>256</v>
+      </c>
+      <c r="J46" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30">
+      <c r="A53" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="3">
+        <v>233.9</v>
+      </c>
+      <c r="D55" s="3">
+        <v>99.37</v>
+      </c>
+      <c r="E55" s="3">
+        <v>128.80000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new data on cyder
git-svn-id: file://localhost/tmp/svn2git/svn@3351 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/terasort/data/Data_Mapreduce.xlsx
+++ b/papers/terasort/data/Data_Mapreduce.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="274" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="7240" windowWidth="17100" windowHeight="13180" tabRatio="352" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sierra-FG" sheetId="4" r:id="rId2"/>
-    <sheet name="India-FG" sheetId="3" r:id="rId3"/>
-    <sheet name="old data" sheetId="1" r:id="rId4"/>
-    <sheet name="Sierra_OLD" sheetId="5" r:id="rId5"/>
+    <sheet name="Cyder" sheetId="6" r:id="rId2"/>
+    <sheet name="Sierra-FG" sheetId="4" r:id="rId3"/>
+    <sheet name="India-FG" sheetId="3" r:id="rId4"/>
+    <sheet name="old data" sheetId="1" r:id="rId5"/>
+    <sheet name="Sierra_OLD" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="123">
   <si>
     <t>Queen Bee</t>
   </si>
@@ -374,6 +375,24 @@
   </si>
   <si>
     <t>Reducer failed create o/p</t>
+  </si>
+  <si>
+    <t>8 workers, 256 mb chunk</t>
+  </si>
+  <si>
+    <t>Prepare input files for reducers</t>
+  </si>
+  <si>
+    <t>Input Data size(MB)</t>
+  </si>
+  <si>
+    <t>Chunk phase</t>
+  </si>
+  <si>
+    <t>Time to Start workers)</t>
+  </si>
+  <si>
+    <t>Prepare input files for reducer</t>
   </si>
 </sst>
 </file>
@@ -467,7 +486,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,8 +508,14 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -558,8 +583,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="116">
+  <cellStyleXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -676,8 +725,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="19"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="19" applyAlignment="1">
@@ -788,8 +841,24 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="36" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="116">
+  <cellStyles count="120">
     <cellStyle name="Explanatory Text" xfId="37" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -846,6 +915,8 @@
     <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="19" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="34" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="35" builtinId="18"/>
@@ -904,6 +975,8 @@
     <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -941,7 +1014,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> time per Each worker in Map, Reduce phase vs chunk size </a:t>
+              <a:t> Time per each worker in Map, Reduce phase vs Chunk Size </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1087,11 +1160,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="476940712"/>
-        <c:axId val="476942488"/>
+        <c:axId val="510024552"/>
+        <c:axId val="472110440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="476940712"/>
+        <c:axId val="510024552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1126,13 +1199,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="476942488"/>
+        <c:crossAx val="472110440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="64.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="476942488"/>
+        <c:axId val="472110440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1167,7 +1240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="476940712"/>
+        <c:crossAx val="510024552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1185,6 +1258,1046 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Chunk</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Size VS </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> to Solution </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.225997765725509"/>
+          <c:y val="0.162728894325103"/>
+          <c:w val="0.707316081383988"/>
+          <c:h val="0.771419430235454"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Time to Create Session in Advert</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0000FF"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$16:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$C$16:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0833333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Time Creating Chunks</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$16:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$D$16:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.916666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.483333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.766666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.316666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Time to Start worker</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="800000"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$16:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$E$16:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Time in Map Phase</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$16:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$F$16:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>34.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.417</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Time in Reduce Phase</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$16:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$G$16:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>54.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="510465304"/>
+        <c:axId val="640330136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="510465304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Chunk</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Size (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.392747140640267"/>
+              <c:y val="0.941605839416058"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="640330136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="640330136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to Solution</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>(Minutes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="510465304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="10.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.470649462612794"/>
+          <c:y val="0.147427438358526"/>
+          <c:w val="0.27570090235071"/>
+          <c:h val="0.244317681092783"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> to Solution Vs input Data Size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.222352474476812"/>
+          <c:y val="0.131076923076923"/>
+          <c:w val="0.642113110385916"/>
+          <c:h val="0.674010417928528"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$5:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0833333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$5:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$D$5:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.583333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.916666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$5:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$E$5:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.266666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$5:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$F$5:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.133</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.233</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.817</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.917</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.933</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$5:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$G$5:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.233</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$A$5:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sierra-FG'!$H$5:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.216666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.216666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.216666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.216666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.216666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.216666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="537145096"/>
+        <c:axId val="510287592"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="537145096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>input</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> size MB</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="510287592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="510287592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time to Solution in minutes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="537145096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1390,11 +2503,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="477024808"/>
-        <c:axId val="477027800"/>
+        <c:axId val="467405672"/>
+        <c:axId val="467408664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="477024808"/>
+        <c:axId val="467405672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,12 +2517,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="477027800"/>
+        <c:crossAx val="467408664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="477027800"/>
+        <c:axId val="467408664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,7 +2533,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="477024808"/>
+        <c:crossAx val="467405672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1455,16 +2568,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1478,6 +2591,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1898,10 +3071,433 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="33" thickBot="1">
+      <c r="A1" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="16" thickTop="1">
+      <c r="A2" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+    </row>
+    <row r="4" spans="1:9" ht="57" thickBot="1">
+      <c r="A4" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" thickTop="1">
+      <c r="A5">
+        <v>128</v>
+      </c>
+      <c r="B5">
+        <v>2.1</v>
+      </c>
+      <c r="C5">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D5">
+        <f>0.5/60</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="E5">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.6</v>
+      </c>
+      <c r="G5">
+        <f>0.5/60</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H5">
+        <v>1.367</v>
+      </c>
+      <c r="I5">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="20" thickBot="1">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+    </row>
+    <row r="25" spans="1:9" ht="61" thickTop="1">
+      <c r="A25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+    </row>
+    <row r="26" spans="1:9" ht="57" thickBot="1">
+      <c r="A26" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>30.8</v>
+      </c>
+      <c r="C27">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D27">
+        <v>1.083</v>
+      </c>
+      <c r="E27">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F27">
+        <v>16.47</v>
+      </c>
+      <c r="G27">
+        <v>0.4</v>
+      </c>
+      <c r="H27">
+        <v>12</v>
+      </c>
+      <c r="I27">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>21.37</v>
+      </c>
+      <c r="C28">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D28">
+        <v>0.53</v>
+      </c>
+      <c r="E28">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F28">
+        <v>8.8330000000000002</v>
+      </c>
+      <c r="G28">
+        <f>12/60</f>
+        <v>0.2</v>
+      </c>
+      <c r="H28">
+        <v>11.95</v>
+      </c>
+      <c r="I28">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>64</v>
+      </c>
+      <c r="B29">
+        <v>16.98</v>
+      </c>
+      <c r="C29">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D29">
+        <v>0.25</v>
+      </c>
+      <c r="E29">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F29">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G29">
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H29">
+        <v>11.85</v>
+      </c>
+      <c r="I29">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>128</v>
+      </c>
+      <c r="B30">
+        <v>15.07</v>
+      </c>
+      <c r="C30">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D30">
+        <f>8/60</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E30">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F30">
+        <v>2.93</v>
+      </c>
+      <c r="G30">
+        <f>3/10</f>
+        <v>0.3</v>
+      </c>
+      <c r="H30">
+        <v>11.75</v>
+      </c>
+      <c r="I30">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>256</v>
+      </c>
+      <c r="B31">
+        <v>14.22</v>
+      </c>
+      <c r="C31">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D31">
+        <f>3/60</f>
+        <v>0.05</v>
+      </c>
+      <c r="E31">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F31">
+        <v>2.65</v>
+      </c>
+      <c r="G31">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H31">
+        <v>11.38</v>
+      </c>
+      <c r="I31">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>512</v>
+      </c>
+      <c r="B32">
+        <v>14.62</v>
+      </c>
+      <c r="C32">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D32">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E32">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F32" s="44">
+        <v>2.35</v>
+      </c>
+      <c r="G32">
+        <f>0.5/60</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H32">
+        <v>12.1</v>
+      </c>
+      <c r="I32">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>1024</v>
+      </c>
+      <c r="C33">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="E33">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="I33">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1993,13 +3589,16 @@
         <v>9.2170000000000005</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <f>6/60</f>
+        <v>0.1</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <f>3/60</f>
+        <v>0.05</v>
       </c>
       <c r="E5">
-        <v>16</v>
+        <f>16/60</f>
+        <v>0.26666666666666666</v>
       </c>
       <c r="F5" s="33">
         <v>2.133</v>
@@ -2008,7 +3607,8 @@
         <v>6.2329999999999997</v>
       </c>
       <c r="H5">
-        <v>13</v>
+        <f t="shared" ref="H5:H10" si="0">13/60</f>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I5" t="s">
         <v>81</v>
@@ -2033,13 +3633,16 @@
         <v>10.220000000000001</v>
       </c>
       <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
+        <f>6/60</f>
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="44">
+        <f>9/60</f>
+        <v>0.15</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F6" s="33">
         <v>2.2330000000000001</v>
@@ -2048,7 +3651,8 @@
         <v>7.05</v>
       </c>
       <c r="H6">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I6" t="s">
         <v>82</v>
@@ -2073,13 +3677,16 @@
         <v>16.78</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <f>6/60</f>
+        <v>0.1</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <f>20/60</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F7" s="33">
         <v>3.8170000000000002</v>
@@ -2088,7 +3695,8 @@
         <v>11.82</v>
       </c>
       <c r="H7">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I7">
         <v>64</v>
@@ -2113,13 +3721,16 @@
         <v>25.62</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <f>6/60</f>
+        <v>0.1</v>
       </c>
       <c r="D8">
-        <v>40</v>
+        <f>40/60</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F8" s="33">
         <v>4.9169999999999998</v>
@@ -2128,7 +3739,8 @@
         <v>19.27</v>
       </c>
       <c r="H8">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I8">
         <v>128</v>
@@ -2153,13 +3765,16 @@
         <v>33.770000000000003</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <f>6/60</f>
+        <v>0.1</v>
       </c>
       <c r="D9">
-        <v>95</v>
+        <f>95/60</f>
+        <v>1.5833333333333333</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F9" s="33">
         <v>9.9329999999999998</v>
@@ -2168,7 +3783,8 @@
         <v>21.37</v>
       </c>
       <c r="H9">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I9">
         <v>256</v>
@@ -2193,13 +3809,16 @@
         <v>58</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D10">
-        <v>175</v>
+        <f>175/60</f>
+        <v>2.9166666666666665</v>
       </c>
       <c r="E10">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F10" s="33">
         <v>17.77</v>
@@ -2208,7 +3827,8 @@
         <v>36.5</v>
       </c>
       <c r="H10">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I10">
         <v>512</v>
@@ -2278,16 +3898,19 @@
         <v>32</v>
       </c>
       <c r="B16">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C16" s="38">
-        <v>6</v>
+        <f>6/60</f>
+        <v>0.1</v>
       </c>
       <c r="D16" s="38">
-        <v>357</v>
+        <f>357/60</f>
+        <v>5.95</v>
       </c>
       <c r="E16" s="38">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F16" s="39">
         <v>34.979999999999997</v>
@@ -2296,7 +3919,8 @@
         <v>54.42</v>
       </c>
       <c r="H16" s="38">
-        <v>13</v>
+        <f>13/60</f>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I16" s="38">
         <v>512</v>
@@ -2321,13 +3945,16 @@
         <v>58</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D17">
-        <v>175</v>
+        <f>175/60</f>
+        <v>2.9166666666666665</v>
       </c>
       <c r="E17">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F17" s="33">
         <v>17.77</v>
@@ -2336,7 +3963,8 @@
         <v>36.5</v>
       </c>
       <c r="H17">
-        <v>13</v>
+        <f>13/60</f>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I17">
         <v>512</v>
@@ -2361,13 +3989,16 @@
         <v>40.17</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D18">
-        <v>89</v>
+        <f>89/60</f>
+        <v>1.4833333333333334</v>
       </c>
       <c r="E18">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F18" s="33">
         <v>10.92</v>
@@ -2376,7 +4007,8 @@
         <v>27</v>
       </c>
       <c r="H18">
-        <v>13</v>
+        <f>13/60</f>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I18">
         <v>512</v>
@@ -2401,13 +4033,16 @@
         <v>31.77</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D19">
-        <v>46</v>
+        <f>46/60</f>
+        <v>0.76666666666666672</v>
       </c>
       <c r="E19">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F19" s="33">
         <v>5.4169999999999998</v>
@@ -2416,7 +4051,8 @@
         <v>24.8</v>
       </c>
       <c r="H19">
-        <v>13</v>
+        <f>13/60</f>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I19">
         <v>512</v>
@@ -2441,13 +4077,16 @@
         <v>31.7</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D20">
-        <v>19</v>
+        <f>19/60</f>
+        <v>0.31666666666666665</v>
       </c>
       <c r="E20">
-        <v>15</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="F20" s="33">
         <v>4.5999999999999996</v>
@@ -2456,7 +4095,8 @@
         <v>25.9</v>
       </c>
       <c r="H20">
-        <v>13</v>
+        <f>13/60</f>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I20">
         <v>512</v>
@@ -2970,11 +4610,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -3220,7 +4860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F43"/>
   <sheetViews>
@@ -3515,7 +5155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>

</xml_diff>

<commit_message>
new graphs and data on cyder
git-svn-id: file://localhost/tmp/svn2git/svn@3353 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/terasort/data/Data_Mapreduce.xlsx
+++ b/papers/terasort/data/Data_Mapreduce.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7240" windowWidth="17100" windowHeight="13180" tabRatio="352" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1540" yWindow="0" windowWidth="26120" windowHeight="17520" tabRatio="352" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="129">
   <si>
     <t>Queen Bee</t>
   </si>
@@ -393,6 +393,24 @@
   </si>
   <si>
     <t>Prepare input files for reducer</t>
+  </si>
+  <si>
+    <t>Varying Num of reduces</t>
+  </si>
+  <si>
+    <t>Constant Input Data size(4GB),Number of workers=8, Chunk Size=256</t>
+  </si>
+  <si>
+    <t>Num Of Reduces</t>
+  </si>
+  <si>
+    <t>Varying Num of workers</t>
+  </si>
+  <si>
+    <t>Num Of workers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constant Input Data size(4GB),Number of workers=8, Chunk Size=256, Nu, of reduces=8 </t>
   </si>
 </sst>
 </file>
@@ -608,7 +626,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="120">
+  <cellStyleXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -647,6 +665,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -858,7 +888,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="120">
+  <cellStyles count="132">
     <cellStyle name="Explanatory Text" xfId="37" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -917,6 +947,12 @@
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="19" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="34" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="35" builtinId="18"/>
@@ -977,6 +1013,12 @@
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -986,6 +1028,2221 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time Vs Input Data</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Master create session</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$C$5:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Chunk Phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$D$5:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.00833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Starting Workers Time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$E$5:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Map phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$F$5:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.083</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.533</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.483</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Prepare Input Files Time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$G$5:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.00833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Reduce Phase Time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$H$5:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.367</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.733</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.533</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Quitting workers Time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$I$5:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="494978248"/>
+        <c:axId val="638789240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="494978248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Input Size in MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="638789240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="638789240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Minutes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="494978248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr i="1"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TIme</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Vs Chunk Size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Master create session</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$C$35:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Chunk Phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$D$35:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.083</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.133333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Starting Workers Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$E$35:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Map phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$F$35:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.833</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Prepare Input Files Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$G$35:$G$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00833333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Reduce Phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$H$35:$H$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Quitting workers Time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$I$35:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="522230824"/>
+        <c:axId val="522236072"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="522230824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Chunk</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Size In MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="522236072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="522236072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in Minutes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="522230824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time VS Num of Reduces</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16015129995543"/>
+          <c:y val="0.0938458513973532"/>
+          <c:w val="0.720077865266842"/>
+          <c:h val="0.822469378827647"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Master create session </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$55:$A$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$C$55:$C$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Chunk Phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$55:$A$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$D$55:$D$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0666666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Starting Workers Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$55:$A$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$E$55:$E$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Map phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$55:$A$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$F$55:$F$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.633</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Prepare Input Files Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$55:$A$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$G$55:$G$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Reduce Phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$55:$A$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$H$55:$H$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>41.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Quitting workers Time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$55:$A$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$I$55:$I$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="506701240"/>
+        <c:axId val="506595240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="506701240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="506595240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="506595240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in Minutes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="506701240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time Vs Num of Workers</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Master create session </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$80:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$C$80:$C$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00833333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Chunk Phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$80:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$D$80:$D$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0666666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Starting Workers Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$80:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$E$80:$E$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0666666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Map phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$80:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$F$80:$F$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.883</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Prepare Input Files Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$80:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$G$80:$G$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Reduce Phase Time </c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$80:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$H$80:$H$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>21.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Quitting workers Time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Cyder!$A$80:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cyder!$I$80:$I$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0333333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="603611032"/>
+        <c:axId val="529566408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="603611032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="529566408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="529566408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in Minutes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="603611032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1160,11 +3417,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="510024552"/>
-        <c:axId val="472110440"/>
+        <c:axId val="535994360"/>
+        <c:axId val="522257592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="510024552"/>
+        <c:axId val="535994360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1199,13 +3456,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="472110440"/>
+        <c:crossAx val="522257592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="64.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="472110440"/>
+        <c:axId val="522257592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,7 +3497,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="510024552"/>
+        <c:crossAx val="535994360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1257,7 +3514,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1641,11 +3898,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="510465304"/>
-        <c:axId val="640330136"/>
+        <c:axId val="522758696"/>
+        <c:axId val="522991736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="510465304"/>
+        <c:axId val="522758696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1686,7 +3943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="640330136"/>
+        <c:crossAx val="522991736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1694,7 +3951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="640330136"/>
+        <c:axId val="522991736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1737,7 +3994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="510465304"/>
+        <c:crossAx val="522758696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
@@ -1775,7 +4032,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1820,8 +4077,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.222352474476812"/>
-          <c:y val="0.131076923076923"/>
+          <c:x val="0.318978189459446"/>
+          <c:y val="0.13387014472353"/>
           <c:w val="0.642113110385916"/>
           <c:h val="0.674010417928528"/>
         </c:manualLayout>
@@ -1833,6 +4090,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Master create session </c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
@@ -1892,6 +4152,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Chunk Phase Time </c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
@@ -1951,6 +4214,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Starting Workers Time </c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
@@ -2010,6 +4276,9 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>Map phase Time </c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
@@ -2069,6 +4338,9 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:v>Reduce Phase Time </c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
@@ -2128,6 +4400,9 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:tx>
+            <c:v>Quitting workers Time</c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
@@ -2194,11 +4469,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="537145096"/>
-        <c:axId val="510287592"/>
+        <c:axId val="535982216"/>
+        <c:axId val="536536824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="537145096"/>
+        <c:axId val="535982216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2237,7 +4512,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="510287592"/>
+        <c:crossAx val="536536824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2245,7 +4520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="510287592"/>
+        <c:axId val="536536824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,21 +4543,37 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0610456016617555"/>
+              <c:y val="0.578417278845731"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="537145096"/>
+        <c:crossAx val="535982216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0199386503067485"/>
+          <c:y val="0.136900321119078"/>
+          <c:w val="0.213358582078381"/>
+          <c:h val="0.370761477892187"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2297,7 +4588,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2503,11 +4794,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="467405672"/>
-        <c:axId val="467408664"/>
+        <c:axId val="523127544"/>
+        <c:axId val="536601864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="467405672"/>
+        <c:axId val="523127544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2517,12 +4808,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="467408664"/>
+        <c:crossAx val="536601864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="467408664"/>
+        <c:axId val="536601864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2533,7 +4824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="467405672"/>
+        <c:crossAx val="523127544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2568,6 +4859,131 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>819150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>774700</xdr:colOff>
       <xdr:row>30</xdr:row>
@@ -2598,16 +5014,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2628,16 +5044,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2659,7 +5075,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3071,10 +5487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C80" sqref="C80:I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3107,9 +5523,7 @@
         <v>49</v>
       </c>
       <c r="C2" s="38"/>
-      <c r="D2" s="49" t="s">
-        <v>75</v>
-      </c>
+      <c r="D2" s="49"/>
       <c r="E2" s="38"/>
       <c r="F2" s="50"/>
       <c r="G2" s="51"/>
@@ -3166,7 +5580,7 @@
         <v>2.1</v>
       </c>
       <c r="C5">
-        <f>1/60</f>
+        <f t="shared" ref="C5:C11" si="0">1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="D5">
@@ -3188,7 +5602,7 @@
         <v>1.367</v>
       </c>
       <c r="I5">
-        <f>2/60</f>
+        <f t="shared" ref="I5:I11" si="1">2/60</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -3196,294 +5610,838 @@
       <c r="A6">
         <v>256</v>
       </c>
+      <c r="B6">
+        <v>2.85</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D6">
+        <f>0.5/60</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="E6">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f>0.5/60</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H6">
+        <v>1.7330000000000001</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
         <v>512</v>
       </c>
+      <c r="B7">
+        <v>3.7</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D7">
+        <f>0.5/60</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="E7">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F7">
+        <v>1.083</v>
+      </c>
+      <c r="G7">
+        <f>0.5/60</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H7">
+        <v>2.5</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
         <v>1024</v>
       </c>
+      <c r="B8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D8">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="E8">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F8">
+        <v>1.35</v>
+      </c>
+      <c r="G8">
+        <f>0.5/60</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H8">
+        <v>3.5329999999999999</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
         <v>2048</v>
       </c>
+      <c r="B9">
+        <v>8.0169999999999995</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D9">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E9">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F9">
+        <v>1.5329999999999999</v>
+      </c>
+      <c r="G9">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H9">
+        <v>6.3</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
         <v>4096</v>
       </c>
+      <c r="B10">
+        <v>14.22</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D10">
+        <f>3/60</f>
+        <v>0.05</v>
+      </c>
+      <c r="E10">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F10">
+        <v>2.65</v>
+      </c>
+      <c r="G10">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H10">
+        <v>11.38</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
         <v>8192</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="20" thickBot="1">
-      <c r="A24" s="1" t="s">
+      <c r="B11">
+        <v>32.28</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D11" s="44">
+        <f>9/60</f>
+        <v>0.15</v>
+      </c>
+      <c r="E11">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F11">
+        <v>7.4829999999999997</v>
+      </c>
+      <c r="G11">
+        <f>3/60</f>
+        <v>0.05</v>
+      </c>
+      <c r="H11">
+        <v>24.5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="20" thickBot="1">
+      <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-    </row>
-    <row r="25" spans="1:9" ht="61" thickTop="1">
-      <c r="A25" s="5" t="s">
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+    </row>
+    <row r="33" spans="1:9" ht="61" thickTop="1">
+      <c r="A33" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-    </row>
-    <row r="26" spans="1:9" ht="57" thickBot="1">
-      <c r="A26" s="8" t="s">
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+    </row>
+    <row r="34" spans="1:9" ht="57" thickBot="1">
+      <c r="A34" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B34" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D34" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E34" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F34" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G34" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H34" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I34" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27">
+    <row r="35" spans="1:9">
+      <c r="A35">
         <v>16</v>
       </c>
-      <c r="B27">
+      <c r="B35">
         <v>30.8</v>
       </c>
-      <c r="C27">
+      <c r="C35">
+        <f t="shared" ref="C35:C41" si="2">1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D35">
+        <v>1.083</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ref="E35:E41" si="3">1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F35">
+        <v>16.47</v>
+      </c>
+      <c r="G35">
+        <v>0.4</v>
+      </c>
+      <c r="H35">
+        <v>12</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ref="I35:I41" si="4">2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>21.37</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D36">
+        <v>0.53</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F36">
+        <v>8.8330000000000002</v>
+      </c>
+      <c r="G36">
+        <f>12/60</f>
+        <v>0.2</v>
+      </c>
+      <c r="H36">
+        <v>11.95</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>64</v>
+      </c>
+      <c r="B37">
+        <v>16.98</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D37">
+        <v>0.25</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F37">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G37">
+        <f>5/60</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H37">
+        <v>11.85</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38">
+        <v>128</v>
+      </c>
+      <c r="B38">
+        <v>15.07</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D38">
+        <f>8/60</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F38">
+        <v>2.93</v>
+      </c>
+      <c r="G38">
+        <f>3/10</f>
+        <v>0.3</v>
+      </c>
+      <c r="H38">
+        <v>11.75</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39">
+        <v>256</v>
+      </c>
+      <c r="B39">
+        <v>14.22</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D39">
+        <f>3/60</f>
+        <v>0.05</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F39">
+        <v>2.65</v>
+      </c>
+      <c r="G39">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="D27">
-        <v>1.083</v>
-      </c>
-      <c r="E27">
+      <c r="H39">
+        <v>11.38</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40">
+        <v>512</v>
+      </c>
+      <c r="B40">
+        <v>14.62</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D40">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F40" s="44">
+        <v>2.35</v>
+      </c>
+      <c r="G40">
+        <f>0.5/60</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H40">
+        <v>12.1</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41">
+        <v>1024</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="20" thickBot="1">
+      <c r="A52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F52" s="33"/>
+      <c r="G52" s="33"/>
+    </row>
+    <row r="53" spans="1:9" ht="61" thickTop="1">
+      <c r="A53" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
+    </row>
+    <row r="54" spans="1:9" ht="57" thickBot="1">
+      <c r="A54" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55">
+        <v>43.27</v>
+      </c>
+      <c r="C55">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="F27">
-        <v>16.47</v>
-      </c>
-      <c r="G27">
-        <v>0.4</v>
-      </c>
-      <c r="H27">
-        <v>12</v>
-      </c>
-      <c r="I27">
+      <c r="D55">
+        <f>4/60</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E55">
+        <f>3/60</f>
+        <v>0.05</v>
+      </c>
+      <c r="F55">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G55">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H55">
+        <v>41.17</v>
+      </c>
+      <c r="I55">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <v>24.23</v>
+      </c>
+      <c r="C56">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28">
-        <v>32</v>
-      </c>
-      <c r="B28">
-        <v>21.37</v>
-      </c>
-      <c r="C28">
+      <c r="D56">
+        <f>4/60</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E56">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F56">
+        <v>2.5830000000000002</v>
+      </c>
+      <c r="G56">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="D28">
-        <v>0.53</v>
-      </c>
-      <c r="E28">
+      <c r="H56">
+        <v>21.42</v>
+      </c>
+      <c r="I56">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57">
+        <v>8</v>
+      </c>
+      <c r="B57">
+        <v>14.22</v>
+      </c>
+      <c r="C57">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="F28">
-        <v>8.8330000000000002</v>
-      </c>
-      <c r="G28">
-        <f>12/60</f>
-        <v>0.2</v>
-      </c>
-      <c r="H28">
-        <v>11.95</v>
-      </c>
-      <c r="I28">
+      <c r="D57">
+        <f>3/60</f>
+        <v>0.05</v>
+      </c>
+      <c r="E57">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29">
-        <v>64</v>
-      </c>
-      <c r="B29">
-        <v>16.98</v>
-      </c>
-      <c r="C29">
+      <c r="F57">
+        <v>2.65</v>
+      </c>
+      <c r="G57">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="D29">
-        <v>0.25</v>
-      </c>
-      <c r="E29">
+      <c r="H57">
+        <v>11.38</v>
+      </c>
+      <c r="I57">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58">
+        <v>16</v>
+      </c>
+      <c r="B58">
+        <v>16.02</v>
+      </c>
+      <c r="C58">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="F29">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="G29">
+      <c r="D58">
+        <f>4/60</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E58">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F58">
+        <v>2.633</v>
+      </c>
+      <c r="G58">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H58">
+        <v>13.17</v>
+      </c>
+      <c r="I58">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59">
+        <v>32</v>
+      </c>
+      <c r="B59">
+        <v>16.88</v>
+      </c>
+      <c r="C59">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D59">
+        <f>4/60</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E59">
+        <f>3/60</f>
+        <v>0.05</v>
+      </c>
+      <c r="F59">
+        <v>2.95</v>
+      </c>
+      <c r="G59">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H59">
+        <v>13.67</v>
+      </c>
+      <c r="I59">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="20" thickBot="1">
+      <c r="A77" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F77" s="33"/>
+      <c r="G77" s="33"/>
+    </row>
+    <row r="78" spans="1:9" ht="76" thickTop="1">
+      <c r="A78" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F78" s="33"/>
+      <c r="G78" s="33"/>
+    </row>
+    <row r="79" spans="1:9" ht="57" thickBot="1">
+      <c r="A79" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F79" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G79" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H79" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80">
+        <v>4</v>
+      </c>
+      <c r="B80">
+        <v>25.37</v>
+      </c>
+      <c r="C80">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D80">
         <f>5/60</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H29">
-        <v>11.85</v>
-      </c>
-      <c r="I29">
+      <c r="E80">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30">
-        <v>128</v>
-      </c>
-      <c r="B30">
-        <v>15.07</v>
-      </c>
-      <c r="C30">
+      <c r="F80">
+        <v>3.883</v>
+      </c>
+      <c r="G80">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="D30">
-        <f>8/60</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="E30">
+      <c r="H80">
+        <v>21.27</v>
+      </c>
+      <c r="I80">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81">
+        <v>8</v>
+      </c>
+      <c r="B81">
+        <v>14.22</v>
+      </c>
+      <c r="C81">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="F30">
-        <v>2.93</v>
-      </c>
-      <c r="G30">
-        <f>3/10</f>
-        <v>0.3</v>
-      </c>
-      <c r="H30">
-        <v>11.75</v>
-      </c>
-      <c r="I30">
+      <c r="D81">
+        <f>3/60</f>
+        <v>0.05</v>
+      </c>
+      <c r="E81">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31">
-        <v>256</v>
-      </c>
-      <c r="B31">
-        <v>14.22</v>
-      </c>
-      <c r="C31">
+      <c r="F81">
+        <v>2.65</v>
+      </c>
+      <c r="G81">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="D31">
-        <f>3/60</f>
-        <v>0.05</v>
-      </c>
-      <c r="E31">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="F31">
-        <v>2.65</v>
-      </c>
-      <c r="G31">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="H31">
+      <c r="H81">
         <v>11.38</v>
       </c>
-      <c r="I31">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32">
-        <v>512</v>
-      </c>
-      <c r="B32">
-        <v>14.62</v>
-      </c>
-      <c r="C32">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="D32">
+      <c r="I81">
         <f>2/60</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="E32">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="F32" s="44">
-        <v>2.35</v>
-      </c>
-      <c r="G32">
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82">
+        <v>16</v>
+      </c>
+      <c r="B82">
+        <v>14.22</v>
+      </c>
+      <c r="C82">
         <f>0.5/60</f>
         <v>8.3333333333333332E-3</v>
       </c>
-      <c r="H32">
-        <v>12.1</v>
-      </c>
-      <c r="I32">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33">
-        <v>1024</v>
-      </c>
-      <c r="C33">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="E33">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="I33">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
+      <c r="D82">
+        <f>4/60</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E82">
+        <f>4/60</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="F82">
+        <v>2.15</v>
+      </c>
+      <c r="G82">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H82">
+        <v>11.78</v>
+      </c>
+      <c r="I82">
+        <f>2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3496,7 +6454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:H15"/>
     </sheetView>
   </sheetViews>
@@ -4600,7 +7558,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>